<commit_message>
Itens in array, 25 max
</commit_message>
<xml_diff>
--- a/Maps/Excel Map.xlsx
+++ b/Maps/Excel Map.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -409,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ET210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BL35" sqref="BL35"/>
+    <sheetView tabSelected="1" topLeftCell="DJ12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N59" sqref="N59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6093,7 +6093,7 @@
         <f t="shared" si="2"/>
         <v>5652</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="3">
         <f t="shared" si="2"/>
         <v>5656</v>
       </c>
@@ -25112,7 +25112,7 @@
         <v>24596</v>
       </c>
       <c r="G49" s="7">
-        <f t="shared" si="126"/>
+        <f>G48+512</f>
         <v>24600</v>
       </c>
       <c r="H49" s="3">
@@ -25625,8 +25625,8 @@
         <f t="shared" si="125"/>
         <v>25108</v>
       </c>
-      <c r="G50" s="7">
-        <f t="shared" si="126"/>
+      <c r="G50" s="3">
+        <f>G49+512</f>
         <v>25112</v>
       </c>
       <c r="H50" s="3">
@@ -30279,7 +30279,7 @@
         <f t="shared" si="3"/>
         <v>29744</v>
       </c>
-      <c r="N59" s="3">
+      <c r="N59" s="7">
         <f t="shared" si="4"/>
         <v>29748</v>
       </c>

</xml_diff>